<commit_message>
third commit with pass and fail ss report
</commit_message>
<xml_diff>
--- a/src/test/resources/Testbook.xlsx
+++ b/src/test/resources/Testbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onkar Kolkur\eclipse-workspace\Auto_Framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2EC5E3-FB59-486E-8198-9E5A18AF66C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B742145E-C920-4B6B-A98B-1753D08390A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mail ID</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Happy@1199</t>
+  </si>
+  <si>
+    <t>poojakolkur11@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
@@ -365,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -393,10 +399,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DCABE3F2-BA6A-4563-9172-FDFDD6262468}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{34411463-B339-4490-AF2B-DBC17EA110CC}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{FA878DA0-8722-4D9E-B358-66F1BC4E7BD8}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{99E17315-EAF4-4E0C-9E6C-DACFCBC8A255}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>